<commit_message>
add coverage annotation links to interrupt vplan
Signed-off-by: Steve Richmond <Steve.Richmond@silabs.com>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/SimulationVerificationPlan/interrupts/CV32E40P_interrupts.xlsx
+++ b/verif/CV32E40P/SimulationVerificationPlan/interrupts/CV32E40P_interrupts.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\strichmo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\silabs.com\design\home\strichmo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B92CA1-F235-4F94-976E-231E8E42D007}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="11190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="High-level Feature" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={0C500716-74FF-41A9-9E2E-F6AE3084E2A3}</author>
     <author>tc={BC1BB870-6BEF-4BC4-8FD4-3D9CF0E47BCA}</author>
@@ -43,29 +42,55 @@
     <author>tc={3A65AAB5-516C-486C-93ED-1FA77D4BC523}</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{0C500716-74FF-41A9-9E2E-F6AE3084E2A3}">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The UM actually constrains this to a single clock cycle pulse.  Recommend we update this Feature Decription to match.
 Reply:
     Will constraint this description to a single clock cycle.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="1" shapeId="0" xr:uid="{BC1BB870-6BEF-4BC4-8FD4-3D9CF0E47BCA}">
+    <comment ref="F3" authorId="1" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     I would need some more details here.  How can we know the core has "taken" and interrupt?   What does "taken" mean?
 Reply:
     In both the assertions mentioned in this plan, and in the ISS modeling of the interrupts, irq_ack_o is the signal used as a hint that the core has "taken" and interrupt.  Once this is seen, the assertions will check proper arbitration, enable, etc. and also the ISS will expect the 2nd instruction afterwards to be the first instruction of the winning interrupt (depending on mtvec mode).</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="D7" authorId="2" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Is this really supported?? Can we ignore?
@@ -73,11 +98,20 @@
     The User Manual clearly documents it and a cursory inspection of the RTL indicates that the core does support it.  A single, dedicated self-checking test should be able to cover this.
 Reply:
     Has been addressed in a bootstrap directed test.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="3" shapeId="0" xr:uid="{B5063E1E-F72A-443E-8603-45F80C4143AF}">
+    <comment ref="F11" authorId="3" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Why not check against ISS?
@@ -87,11 +121,20 @@
     ISS can (and is) checking nested interrupts in the directed interrupt test.  I tried the enable_nested_interrupt in riscv-dv and it is broken (doesn't stack the mepc for example).  Is it necessary to add more random testing for nested interrupts?
 Reply:
     Went ahead and extended corev-dv to support this.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="4" shapeId="0" xr:uid="{0878F7E8-522F-411F-8652-CE9509E3997A}">
+    <comment ref="F12" authorId="4" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Why not check against ISS?
@@ -101,11 +144,20 @@
     See above.
 Reply:
     Functionality is checked but in a directed fashion.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="5" shapeId="0" xr:uid="{8F18CFB5-712B-4251-A5D8-F5CB4694E4E1}">
+    <comment ref="F13" authorId="5" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Why not check against ISS?
@@ -115,11 +167,20 @@
     See above.  Functionality is checked but in a directed fashion.
 Reply:
     Extended corev-dv to support random nested irq handlers.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="6" shapeId="0" xr:uid="{BB0B890D-2754-494D-8562-98355052E8A1}">
+    <comment ref="G14" authorId="6" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Do we need a DSC test for this?  Won't any random test cover this assuming we are checking against the ISS?
@@ -127,31 +188,58 @@
     Yes...just mentioning as a functionality.
 Reply:
     It should be checked by ISS.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="G21" authorId="7" shapeId="0" xr:uid="{E4746BD7-7E1B-49BA-8057-92724CF327A0}">
+    <comment ref="G21" authorId="7" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Do we need a DSC test for this?  Won't any random test cover this assuming we are checking against the ISS?
 Reply:
     Should be covered in random especially with random nested interrupts running now.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D28" authorId="8" shapeId="0" xr:uid="{5A201864-4453-4040-AB3A-756259B8674F}">
+    <comment ref="D28" authorId="8" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     I think the timer is irq_i[7]
 Reply:
     Thanks...fixing the typo.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="9" shapeId="0" xr:uid="{DBF72415-992E-4687-89AA-594D06092EF4}">
+    <comment ref="B36" authorId="9" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     General comment for all the "Interrupt Instruction" features in this DV plan.  This is important and will produce a large, difficult to fill functional coverage model.  Is there a way to use FV to provide exhaustive coverage of this?
@@ -159,11 +247,20 @@
     Coverage reports show all instructions covered here.
 Reply:
     Will leave of functional coverage as defined here.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D71" authorId="10" shapeId="0" xr:uid="{A5AF476F-84B5-40AF-A1B5-D98D67880192}">
+    <comment ref="D71" authorId="10" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This requirement seems untestable for CLINT interrupts.
@@ -171,14 +268,24 @@
     Why is that?
 Reply:
     Will leave as a documented assumption on the interrupt modeling in the verification infrastructure.</t>
+        </r>
       </text>
     </comment>
-    <comment ref="C73" authorId="11" shapeId="0" xr:uid="{3A65AAB5-516C-486C-93ED-1FA77D4BC523}">
+    <comment ref="C73" authorId="11" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     the Pulp tests EM contributed are self-checking.  If an interrupt is serviced properly it should still pass.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -186,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="214">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -606,9 +713,6 @@
     <t>WFI is exitted and normal operation occurs if an enabled interrupt becomes pending</t>
   </si>
   <si>
-    <t xml:space="preserve">WFI is exitted within a certain time period after a </t>
-  </si>
-  <si>
     <t>Exit with global MIE disable</t>
   </si>
   <si>
@@ -1424,12 +1528,68 @@
   </si>
   <si>
     <t>All assertions and modeling of interrupts for checking assume no edges required to qualify an interrupt.</t>
+  </si>
+  <si>
+    <t>DTC "interrupt_test"</t>
+  </si>
+  <si>
+    <t>CG: uvm_pkg.uvm_test_top.env.cov_model.interrupt_covg.cg_irq_entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CG: uvm_pkg.uvm_test_top.env.cov_model.interrupt_covg.cg_irq_entry
+CG: uvm_pkg.uvm_test_top.env.cov_model.interrupt_covg.cg_irq_exit
+</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i.a_irq_id_o_mstatus_mie_enabled</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i,gen_wfi_cov[*].c_wfi_wake_mstatus_mie_*</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i,gen_wfi_cov[*].c_wfi_wake_mstatus_mie_0</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i,a_wfi_wake_to_instr_fetch</t>
+  </si>
+  <si>
+    <t>WFI is exitted within a 40 free-running clcoks after a valid wakeup event</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i,a_wfi_assert_core_sleep_o</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i,a_irq_arb</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i.gen_irq_cov[*].c_irq_masked_then_enabled</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i.gen_irq_cov[*].c_irq_taken</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i.a_irq_id_o_mie_enabled</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i.a_mip_not_reserved</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i.a_mip_irq_i</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i.a_irq_id_o_not_reserved</t>
+  </si>
+  <si>
+    <t>DTC "interrupt_bootstrap_test"</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32_tb.dut_wrap.cv32e40p_wrapper_i.core_i.interrupt_assert_i.a_irq_ack_o_pulse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -1525,7 +1685,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1571,10 +1731,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2073,13 +2236,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
@@ -2092,7 +2255,7 @@
     <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="41.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="116.140625" style="1" customWidth="1"/>
     <col min="10" max="1023" width="17" style="1"/>
     <col min="1024" max="1024" width="9.140625" style="1" customWidth="1"/>
   </cols>
@@ -2151,7 +2314,9 @@
       <c r="H2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" ht="72">
       <c r="A3" s="13" t="s">
@@ -2164,7 +2329,7 @@
         <v>46</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>54</v>
@@ -2176,7 +2341,7 @@
         <v>26</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I3" s="6"/>
     </row>
@@ -2203,7 +2368,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I4" s="6"/>
     </row>
@@ -2232,7 +2397,9 @@
       <c r="H5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A6" s="13" t="s">
@@ -2259,7 +2426,9 @@
       <c r="H6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A7" s="13" t="s">
@@ -2271,7 +2440,7 @@
       <c r="C7" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -2286,7 +2455,9 @@
       <c r="H7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="6" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="8" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A8" s="13" t="s">
@@ -2311,7 +2482,7 @@
         <v>23</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I8" s="6"/>
     </row>
@@ -2338,9 +2509,11 @@
         <v>23</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="10" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A10" s="13" t="s">
@@ -2365,9 +2538,11 @@
         <v>23</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="11" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A11" s="13" t="s">
@@ -2394,7 +2569,9 @@
       <c r="H11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="12" spans="1:9" s="5" customFormat="1" ht="72">
       <c r="A12" s="13" t="s">
@@ -2421,7 +2598,9 @@
       <c r="H12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="13" spans="1:9" s="5" customFormat="1" ht="72">
       <c r="A13" s="13" t="s">
@@ -2448,7 +2627,9 @@
       <c r="H13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="14" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A14" s="13" t="s">
@@ -2475,7 +2656,9 @@
       <c r="H14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="15" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A15" s="13" t="s">
@@ -2502,7 +2685,9 @@
       <c r="H15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="16" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A16" s="13" t="s">
@@ -2529,7 +2714,9 @@
       <c r="H16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="6" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="17" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A17" s="13" t="s">
@@ -2556,7 +2743,9 @@
       <c r="H17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="I17" s="6" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="18" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A18" s="13" t="s">
@@ -2581,9 +2770,11 @@
         <v>23</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="19" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A19" s="13" t="s">
@@ -2610,7 +2801,9 @@
       <c r="H19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="6"/>
+      <c r="I19" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="20" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A20" s="13" t="s">
@@ -2635,9 +2828,11 @@
         <v>23</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A21" s="13" t="s">
@@ -2664,7 +2859,9 @@
       <c r="H21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="22" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A22" s="13" t="s">
@@ -2680,7 +2877,7 @@
         <v>123</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>16</v>
@@ -2691,7 +2888,9 @@
       <c r="H22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="23" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A23" s="13" t="s">
@@ -2718,7 +2917,9 @@
       <c r="H23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="6"/>
+      <c r="I23" s="6" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="24" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A24" s="13" t="s">
@@ -2745,7 +2946,9 @@
       <c r="H24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="6" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="25" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A25" s="13" t="s">
@@ -2772,7 +2975,9 @@
       <c r="H25" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="6"/>
+      <c r="I25" s="6" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="26" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A26" s="13" t="s">
@@ -2799,7 +3004,9 @@
       <c r="H26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="6"/>
+      <c r="I26" s="6" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="27" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A27" s="13" t="s">
@@ -2826,7 +3033,9 @@
       <c r="H27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="6"/>
+      <c r="I27" s="6" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="28" spans="1:9" s="5" customFormat="1" ht="57.75">
       <c r="A28" s="13" t="s">
@@ -2839,7 +3048,7 @@
         <v>116</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>117</v>
@@ -2853,7 +3062,9 @@
       <c r="H28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="6"/>
+      <c r="I28" s="6" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="29" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A29" s="13" t="s">
@@ -2878,7 +3089,7 @@
         <v>26</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I29" s="6"/>
     </row>
@@ -2905,7 +3116,7 @@
         <v>26</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I30" s="6"/>
     </row>
@@ -2934,7 +3145,9 @@
       <c r="H31" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="6"/>
+      <c r="I31" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="32" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A32" s="13" t="s">
@@ -2950,7 +3163,7 @@
         <v>138</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>22</v>
@@ -2961,7 +3174,9 @@
       <c r="H32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="6"/>
+      <c r="I32" s="6" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="33" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A33" s="13" t="s">
@@ -2971,13 +3186,13 @@
         <v>127</v>
       </c>
       <c r="C33" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>142</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>16</v>
@@ -2988,7 +3203,9 @@
       <c r="H33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I33" s="6"/>
+      <c r="I33" s="6" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="34" spans="1:9" s="5" customFormat="1" ht="43.5">
       <c r="A34" s="13" t="s">
@@ -2998,13 +3215,13 @@
         <v>127</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>10</v>
@@ -3015,7 +3232,9 @@
       <c r="H34" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="6"/>
+      <c r="I34" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="35" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A35" s="13" t="s">
@@ -3025,13 +3244,13 @@
         <v>127</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>16</v>
@@ -3042,7 +3261,9 @@
       <c r="H35" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I35" s="6"/>
+      <c r="I35" s="6" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="36" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A36" s="13" t="s">
@@ -3052,7 +3273,7 @@
         <v>124</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>125</v>
@@ -3069,7 +3290,9 @@
       <c r="H36" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I36" s="6"/>
+      <c r="I36" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="37" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A37" s="13" t="s">
@@ -3079,7 +3302,7 @@
         <v>124</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>125</v>
@@ -3096,7 +3319,9 @@
       <c r="H37" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I37" s="6"/>
+      <c r="I37" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="38" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A38" s="13" t="s">
@@ -3106,7 +3331,7 @@
         <v>124</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>125</v>
@@ -3123,7 +3348,9 @@
       <c r="H38" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I38" s="6"/>
+      <c r="I38" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="39" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A39" s="13" t="s">
@@ -3133,7 +3360,7 @@
         <v>124</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>125</v>
@@ -3150,7 +3377,9 @@
       <c r="H39" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I39" s="6"/>
+      <c r="I39" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="40" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A40" s="13" t="s">
@@ -3160,7 +3389,7 @@
         <v>124</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>125</v>
@@ -3177,7 +3406,9 @@
       <c r="H40" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I40" s="6"/>
+      <c r="I40" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="41" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A41" s="13" t="s">
@@ -3187,7 +3418,7 @@
         <v>124</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>125</v>
@@ -3204,7 +3435,9 @@
       <c r="H41" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="6"/>
+      <c r="I41" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="42" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A42" s="13" t="s">
@@ -3214,7 +3447,7 @@
         <v>124</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>125</v>
@@ -3231,7 +3464,9 @@
       <c r="H42" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I42" s="6"/>
+      <c r="I42" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="43" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A43" s="13" t="s">
@@ -3241,7 +3476,7 @@
         <v>124</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>125</v>
@@ -3258,7 +3493,9 @@
       <c r="H43" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I43" s="6"/>
+      <c r="I43" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="44" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A44" s="13" t="s">
@@ -3268,7 +3505,7 @@
         <v>124</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>125</v>
@@ -3285,7 +3522,9 @@
       <c r="H44" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I44" s="6"/>
+      <c r="I44" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="45" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A45" s="13" t="s">
@@ -3295,7 +3534,7 @@
         <v>124</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>125</v>
@@ -3312,7 +3551,9 @@
       <c r="H45" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I45" s="6"/>
+      <c r="I45" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="46" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A46" s="13" t="s">
@@ -3322,7 +3563,7 @@
         <v>124</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>125</v>
@@ -3339,7 +3580,9 @@
       <c r="H46" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I46" s="6"/>
+      <c r="I46" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="47" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A47" s="13" t="s">
@@ -3349,7 +3592,7 @@
         <v>124</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>125</v>
@@ -3366,7 +3609,9 @@
       <c r="H47" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I47" s="6"/>
+      <c r="I47" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="48" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A48" s="13" t="s">
@@ -3376,7 +3621,7 @@
         <v>124</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>125</v>
@@ -3393,7 +3638,9 @@
       <c r="H48" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I48" s="6"/>
+      <c r="I48" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="49" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A49" s="13" t="s">
@@ -3403,7 +3650,7 @@
         <v>124</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>125</v>
@@ -3420,7 +3667,9 @@
       <c r="H49" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I49" s="6"/>
+      <c r="I49" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="50" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A50" s="13" t="s">
@@ -3430,7 +3679,7 @@
         <v>124</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>125</v>
@@ -3447,7 +3696,9 @@
       <c r="H50" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I50" s="6"/>
+      <c r="I50" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="51" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A51" s="13" t="s">
@@ -3457,7 +3708,7 @@
         <v>124</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>125</v>
@@ -3474,7 +3725,9 @@
       <c r="H51" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I51" s="6"/>
+      <c r="I51" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="52" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A52" s="13" t="s">
@@ -3484,7 +3737,7 @@
         <v>124</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>125</v>
@@ -3501,7 +3754,9 @@
       <c r="H52" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I52" s="6"/>
+      <c r="I52" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="53" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A53" s="13" t="s">
@@ -3511,7 +3766,7 @@
         <v>124</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>125</v>
@@ -3528,7 +3783,9 @@
       <c r="H53" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I53" s="6"/>
+      <c r="I53" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="54" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A54" s="13" t="s">
@@ -3538,7 +3795,7 @@
         <v>124</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>125</v>
@@ -3555,7 +3812,9 @@
       <c r="H54" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I54" s="6"/>
+      <c r="I54" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="55" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A55" s="13" t="s">
@@ -3565,7 +3824,7 @@
         <v>124</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>125</v>
@@ -3582,7 +3841,9 @@
       <c r="H55" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I55" s="6"/>
+      <c r="I55" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="56" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A56" s="13" t="s">
@@ -3592,7 +3853,7 @@
         <v>124</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>125</v>
@@ -3609,7 +3870,9 @@
       <c r="H56" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I56" s="6"/>
+      <c r="I56" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="57" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A57" s="13" t="s">
@@ -3619,7 +3882,7 @@
         <v>124</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>125</v>
@@ -3636,7 +3899,9 @@
       <c r="H57" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I57" s="6"/>
+      <c r="I57" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="58" spans="1:9" s="5" customFormat="1" ht="45">
       <c r="A58" s="13" t="s">
@@ -3646,7 +3911,7 @@
         <v>124</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>125</v>
@@ -3663,7 +3928,9 @@
       <c r="H58" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I58" s="6"/>
+      <c r="I58" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="59" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A59" s="13" t="s">
@@ -3673,7 +3940,7 @@
         <v>124</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>125</v>
@@ -3690,7 +3957,9 @@
       <c r="H59" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I59" s="6"/>
+      <c r="I59" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="60" spans="1:9" s="5" customFormat="1" ht="59.25">
       <c r="A60" s="13" t="s">
@@ -3700,7 +3969,7 @@
         <v>124</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>125</v>
@@ -3717,7 +3986,9 @@
       <c r="H60" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I60" s="6"/>
+      <c r="I60" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="61" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A61" s="13" t="s">
@@ -3727,7 +3998,7 @@
         <v>124</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>125</v>
@@ -3744,7 +4015,9 @@
       <c r="H61" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I61" s="6"/>
+      <c r="I61" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="62" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A62" s="13" t="s">
@@ -3754,7 +4027,7 @@
         <v>124</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>125</v>
@@ -3771,7 +4044,9 @@
       <c r="H62" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I62" s="6"/>
+      <c r="I62" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="63" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A63" s="13" t="s">
@@ -3781,7 +4056,7 @@
         <v>124</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>125</v>
@@ -3798,7 +4073,9 @@
       <c r="H63" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I63" s="6"/>
+      <c r="I63" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="64" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A64" s="13" t="s">
@@ -3808,7 +4085,7 @@
         <v>124</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>125</v>
@@ -3825,7 +4102,9 @@
       <c r="H64" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I64" s="6"/>
+      <c r="I64" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="65" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A65" s="13" t="s">
@@ -3835,7 +4114,7 @@
         <v>124</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>125</v>
@@ -3852,7 +4131,9 @@
       <c r="H65" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I65" s="6"/>
+      <c r="I65" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="66" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A66" s="13" t="s">
@@ -3862,7 +4143,7 @@
         <v>124</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>125</v>
@@ -3879,7 +4160,9 @@
       <c r="H66" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I66" s="6"/>
+      <c r="I66" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="67" spans="1:9" s="5" customFormat="1" ht="44.25">
       <c r="A67" s="13" t="s">
@@ -3889,7 +4172,7 @@
         <v>124</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>125</v>
@@ -3906,7 +4189,9 @@
       <c r="H67" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I67" s="6"/>
+      <c r="I67" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="68" spans="1:9" s="5" customFormat="1" ht="58.5">
       <c r="A68" s="13" t="s">
@@ -3916,7 +4201,7 @@
         <v>124</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>125</v>
@@ -3933,7 +4218,9 @@
       <c r="H68" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I68" s="6"/>
+      <c r="I68" s="6" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="69" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A69" s="13" t="s">
@@ -3943,13 +4230,13 @@
         <v>81</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>16</v>
@@ -3960,7 +4247,9 @@
       <c r="H69" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I69" s="6"/>
+      <c r="I69" s="6" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="70" spans="1:9" s="5" customFormat="1" ht="29.25">
       <c r="A70" s="13" t="s">
@@ -3970,22 +4259,22 @@
         <v>81</v>
       </c>
       <c r="C70" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E70" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D70" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>154</v>
-      </c>
       <c r="F70" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I70" s="6"/>
     </row>
@@ -3994,16 +4283,16 @@
         <v>35</v>
       </c>
       <c r="B71" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C71" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="D71" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F71" s="7" t="s">
         <v>25</v>
@@ -4027,11 +4316,11 @@
         <v>68</v>
       </c>
       <c r="D72" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E72" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E72" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="F72" s="7" t="s">
         <v>16</v>
       </c>
@@ -4039,7 +4328,7 @@
         <v>23</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="I72" s="6"/>
     </row>
@@ -4051,7 +4340,7 @@
         <v>124</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>125</v>
@@ -4068,7 +4357,9 @@
       <c r="H73" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I73" s="6"/>
+      <c r="I73" s="23" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="74" spans="1:9" s="5" customFormat="1">
       <c r="A74" s="6"/>
@@ -4258,17 +4549,17 @@
       <c r="I90" s="6"/>
     </row>
     <row r="91" spans="1:9" s="8" customFormat="1">
-      <c r="A91" s="21" t="s">
+      <c r="A91" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="21"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
-      <c r="G91" s="21"/>
-      <c r="H91" s="21"/>
-      <c r="I91" s="21"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4280,7 +4571,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DONOTDELETE!$E$3:$E$7</xm:f>
           </x14:formula1>
@@ -4289,7 +4580,7 @@
           </x14:formula2>
           <xm:sqref>H2:H90</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DONOTDELETE!$C$3:$C$10</xm:f>
           </x14:formula1>
@@ -4298,7 +4589,7 @@
           </x14:formula2>
           <xm:sqref>G2:G90</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$10</xm:f>
           </x14:formula1>
@@ -4314,7 +4605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -4425,7 +4716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4496,7 +4787,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>